<commit_message>
Add link to video
</commit_message>
<xml_diff>
--- a/Excel_Challenge_434 - Generate the Column Headers Matrix.xlsx
+++ b/Excel_Challenge_434 - Generate the Column Headers Matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="203" documentId="8_{CD3551B2-3A5A-4B49-A231-7D9319C3D9C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E1573DD6-17BB-42D8-9556-8434CBA55A43}"/>
+  <xr:revisionPtr revIDLastSave="204" documentId="8_{CD3551B2-3A5A-4B49-A231-7D9319C3D9C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64741896-B7B5-4650-A75C-412B56148670}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="1665" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="109">
   <si>
     <t>A</t>
   </si>
@@ -405,6 +405,9 @@
   </si>
   <si>
     <t>EF</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=tm2sujY-k-M</t>
   </si>
 </sst>
 </file>
@@ -727,8 +730,8 @@
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
 <rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
   <rv s="0">
+    <v>1</v>
     <v>2</v>
-    <v>1</v>
     <v>19</v>
   </rv>
 </rvData>
@@ -737,8 +740,8 @@
 <file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
 <rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
   <s t="_error">
+    <k n="argument" t="s"/>
     <k n="errorType" t="i"/>
-    <k n="argument" t="s"/>
     <k n="subType" t="i"/>
   </s>
 </rvStructures>
@@ -1007,15 +1010,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:Q126"/>
+  <dimension ref="A1:Q126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M50" sqref="M50"/>
+      <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="Q1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1058,7 +1066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1106,7 +1114,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1154,7 +1162,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1202,7 +1210,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1250,7 +1258,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -1298,7 +1306,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -1346,7 +1354,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -1394,7 +1402,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -1442,7 +1450,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -1490,7 +1498,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -1538,7 +1546,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>55</v>
       </c>
@@ -1586,7 +1594,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -1634,7 +1642,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>65</v>
       </c>
@@ -1682,7 +1690,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>70</v>
       </c>
@@ -7029,7 +7037,7 @@
   <dimension ref="A2:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="A5:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Another challenge bites the dust
</commit_message>
<xml_diff>
--- a/Excel_Challenge_434 - Generate the Column Headers Matrix.xlsx
+++ b/Excel_Challenge_434 - Generate the Column Headers Matrix.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="204" documentId="8_{CD3551B2-3A5A-4B49-A231-7D9319C3D9C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64741896-B7B5-4650-A75C-412B56148670}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{735D0903-D295-418A-8FB1-7452FBF50C49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="1665" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11508" yWindow="-12" windowWidth="11544" windowHeight="12264" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{2A8479CA-27B8-4C58-BCA9-075DC8223C5A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
-    <sheet name="Logic" sheetId="2" r:id="rId3"/>
+    <sheet name="MyDrillSolution" sheetId="1" r:id="rId1"/>
+    <sheet name="Solution2" sheetId="4" r:id="rId2"/>
+    <sheet name="Scratch" sheetId="3" r:id="rId3"/>
+    <sheet name="Logic" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="cr">_xlfn.LAMBDA(_xlpm.x,MID("ABCDEFGHIJKLMNOPQRSTUVWXYZ",_xlpm.x,1))</definedName>
@@ -81,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="109">
   <si>
     <t>A</t>
   </si>
@@ -414,7 +416,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -433,6 +435,14 @@
       <b/>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -467,17 +477,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Intro_Hd" xfId="2" xr:uid="{38CF1D9C-E25E-4A42-A7D2-A52202F9E7FF}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{DE752122-A8AE-4ED2-9DAE-BF695B05030C}"/>
@@ -730,8 +743,8 @@
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
 <rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
   <rv s="0">
+    <v>2</v>
     <v>1</v>
-    <v>2</v>
     <v>19</v>
   </rv>
 </rvData>
@@ -740,8 +753,8 @@
 <file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
 <rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
   <s t="_error">
+    <k n="errorType" t="i"/>
     <k n="argument" t="s"/>
-    <k n="errorType" t="i"/>
     <k n="subType" t="i"/>
   </s>
 </rvStructures>
@@ -1012,14 +1025,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q126"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1"/>
+    </sheetView>
+    <sheetView workbookViewId="1">
+      <selection activeCell="A2" sqref="A2:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="Q1" t="s">
+      <c r="Q1" s="3" t="s">
         <v>108</v>
       </c>
     </row>
@@ -3940,18 +3956,1855 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="Q1" r:id="rId1" xr:uid="{28A727F4-EF37-44FD-9340-B1803DAADA8D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61EE3FBE-54E5-4362-98AD-8B622882160D}">
+  <dimension ref="C1:R104"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <selection activeCell="N27" sqref="N27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="N1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="N2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="N3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="N4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C5" s="1" cm="1">
+        <f t="array" ref="C5:C104">_xlfn.SCAN(1,_xlfn.SEQUENCE(100,,0), _xlfn.LAMBDA(_xlpm.a,_xlpm.b,_xlpm.a+_xlpm.b))</f>
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="str">
+        <f>SUBSTITUTE(ADDRESS(1,C5,4),"1","")</f>
+        <v>A</v>
+      </c>
+      <c r="F5" s="1" t="str" cm="1">
+        <f t="array" ref="F5:J24">_xlfn.WRAPCOLS(D5:D104,20)</f>
+        <v>A</v>
+      </c>
+      <c r="G5" s="1" t="str">
+        <v>HC</v>
+      </c>
+      <c r="H5" s="1" t="str">
+        <v>AEO</v>
+      </c>
+      <c r="I5" s="1" t="str">
+        <v>BRK</v>
+      </c>
+      <c r="J5" s="1" t="str">
+        <v>DTQ</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C6" s="1">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1" t="str">
+        <f t="shared" ref="D6:D69" si="0">SUBSTITUTE(ADDRESS(1,C6,4),"1","")</f>
+        <v>B</v>
+      </c>
+      <c r="F6" s="1" t="str">
+        <v>B</v>
+      </c>
+      <c r="G6" s="1" t="str">
+        <v>HX</v>
+      </c>
+      <c r="H6" s="1" t="str">
+        <v>AGD</v>
+      </c>
+      <c r="I6" s="1" t="str">
+        <v>BTT</v>
+      </c>
+      <c r="J6" s="1" t="str">
+        <v>DWT</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C7" s="1">
+        <v>4</v>
+      </c>
+      <c r="D7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>D</v>
+      </c>
+      <c r="F7" s="1" t="str">
+        <v>D</v>
+      </c>
+      <c r="G7" s="1" t="str">
+        <v>IT</v>
+      </c>
+      <c r="H7" s="1" t="str">
+        <v>AHT</v>
+      </c>
+      <c r="I7" s="1" t="str">
+        <v>BWD</v>
+      </c>
+      <c r="J7" s="1" t="str">
+        <v>DZX</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C8" s="1">
+        <v>7</v>
+      </c>
+      <c r="D8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>G</v>
+      </c>
+      <c r="F8" s="1" t="str">
+        <v>G</v>
+      </c>
+      <c r="G8" s="1" t="str">
+        <v>JQ</v>
+      </c>
+      <c r="H8" s="1" t="str">
+        <v>AJK</v>
+      </c>
+      <c r="I8" s="1" t="str">
+        <v>BYO</v>
+      </c>
+      <c r="J8" s="1" t="str">
+        <v>EDC</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C9" s="1">
+        <v>11</v>
+      </c>
+      <c r="D9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>K</v>
+      </c>
+      <c r="F9" s="1" t="str">
+        <v>K</v>
+      </c>
+      <c r="G9" s="1" t="str">
+        <v>KO</v>
+      </c>
+      <c r="H9" s="1" t="str">
+        <v>ALC</v>
+      </c>
+      <c r="I9" s="1" t="str">
+        <v>CBA</v>
+      </c>
+      <c r="J9" s="1" t="str">
+        <v>EGI</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C10" s="1">
+        <v>16</v>
+      </c>
+      <c r="D10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>P</v>
+      </c>
+      <c r="F10" s="1" t="str">
+        <v>P</v>
+      </c>
+      <c r="G10" s="1" t="str">
+        <v>LN</v>
+      </c>
+      <c r="H10" s="1" t="str">
+        <v>AMV</v>
+      </c>
+      <c r="I10" s="1" t="str">
+        <v>CDN</v>
+      </c>
+      <c r="J10" s="1" t="str">
+        <v>EJP</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C11" s="1">
+        <v>22</v>
+      </c>
+      <c r="D11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>V</v>
+      </c>
+      <c r="F11" s="1" t="str">
+        <v>V</v>
+      </c>
+      <c r="G11" s="1" t="str">
+        <v>MN</v>
+      </c>
+      <c r="H11" s="1" t="str">
+        <v>AOP</v>
+      </c>
+      <c r="I11" s="1" t="str">
+        <v>CGB</v>
+      </c>
+      <c r="J11" s="1" t="str">
+        <v>EMX</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C12" s="1">
+        <v>29</v>
+      </c>
+      <c r="D12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>AC</v>
+      </c>
+      <c r="F12" s="1" t="str">
+        <v>AC</v>
+      </c>
+      <c r="G12" s="1" t="str">
+        <v>NO</v>
+      </c>
+      <c r="H12" s="1" t="str">
+        <v>AQK</v>
+      </c>
+      <c r="I12" s="1" t="str">
+        <v>CIQ</v>
+      </c>
+      <c r="J12" s="1" t="str">
+        <v>EQG</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C13" s="1">
+        <v>37</v>
+      </c>
+      <c r="D13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>AK</v>
+      </c>
+      <c r="F13" s="1" t="str">
+        <v>AK</v>
+      </c>
+      <c r="G13" s="1" t="str">
+        <v>OQ</v>
+      </c>
+      <c r="H13" s="1" t="str">
+        <v>ASG</v>
+      </c>
+      <c r="I13" s="1" t="str">
+        <v>CLG</v>
+      </c>
+      <c r="J13" s="1" t="str">
+        <v>ETQ</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C14" s="1">
+        <v>46</v>
+      </c>
+      <c r="D14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>AT</v>
+      </c>
+      <c r="F14" s="1" t="str">
+        <v>AT</v>
+      </c>
+      <c r="G14" s="1" t="str">
+        <v>PT</v>
+      </c>
+      <c r="H14" s="1" t="str">
+        <v>AUD</v>
+      </c>
+      <c r="I14" s="1" t="str">
+        <v>CNX</v>
+      </c>
+      <c r="J14" s="1" t="str">
+        <v>EXB</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C15" s="1">
+        <v>56</v>
+      </c>
+      <c r="D15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>BD</v>
+      </c>
+      <c r="F15" s="1" t="str">
+        <v>BD</v>
+      </c>
+      <c r="G15" s="1" t="str">
+        <v>QX</v>
+      </c>
+      <c r="H15" s="1" t="str">
+        <v>AWB</v>
+      </c>
+      <c r="I15" s="1" t="str">
+        <v>CQP</v>
+      </c>
+      <c r="J15" s="1" t="str">
+        <v>FAN</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="R15" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C16" s="1">
+        <v>67</v>
+      </c>
+      <c r="D16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>BO</v>
+      </c>
+      <c r="F16" s="1" t="str">
+        <v>BO</v>
+      </c>
+      <c r="G16" s="1" t="str">
+        <v>SC</v>
+      </c>
+      <c r="H16" s="1" t="str">
+        <v>AYA</v>
+      </c>
+      <c r="I16" s="1" t="str">
+        <v>CTI</v>
+      </c>
+      <c r="J16" s="1" t="str">
+        <v>FEA</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C17" s="1">
+        <v>79</v>
+      </c>
+      <c r="D17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CA</v>
+      </c>
+      <c r="F17" s="1" t="str">
+        <v>CA</v>
+      </c>
+      <c r="G17" s="1" t="str">
+        <v>TI</v>
+      </c>
+      <c r="H17" s="1" t="str">
+        <v>BAA</v>
+      </c>
+      <c r="I17" s="1" t="str">
+        <v>CWC</v>
+      </c>
+      <c r="J17" s="1" t="str">
+        <v>FHO</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="R17" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C18" s="1">
+        <v>92</v>
+      </c>
+      <c r="D18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CN</v>
+      </c>
+      <c r="F18" s="1" t="str">
+        <v>CN</v>
+      </c>
+      <c r="G18" s="1" t="str">
+        <v>UP</v>
+      </c>
+      <c r="H18" s="1" t="str">
+        <v>BCB</v>
+      </c>
+      <c r="I18" s="1" t="str">
+        <v>CYX</v>
+      </c>
+      <c r="J18" s="1" t="str">
+        <v>FLD</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C19" s="1">
+        <v>106</v>
+      </c>
+      <c r="D19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>DB</v>
+      </c>
+      <c r="F19" s="1" t="str">
+        <v>DB</v>
+      </c>
+      <c r="G19" s="1" t="str">
+        <v>VX</v>
+      </c>
+      <c r="H19" s="1" t="str">
+        <v>BED</v>
+      </c>
+      <c r="I19" s="1" t="str">
+        <v>DBT</v>
+      </c>
+      <c r="J19" s="1" t="str">
+        <v>FOT</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="R19" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C20" s="1">
+        <v>121</v>
+      </c>
+      <c r="D20" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>DQ</v>
+      </c>
+      <c r="F20" s="1" t="str">
+        <v>DQ</v>
+      </c>
+      <c r="G20" s="1" t="str">
+        <v>XG</v>
+      </c>
+      <c r="H20" s="1" t="str">
+        <v>BGG</v>
+      </c>
+      <c r="I20" s="1" t="str">
+        <v>DEQ</v>
+      </c>
+      <c r="J20" s="1" t="str">
+        <v>FSK</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q20" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="R20" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C21" s="1">
+        <v>137</v>
+      </c>
+      <c r="D21" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>EG</v>
+      </c>
+      <c r="F21" s="1" t="str">
+        <v>EG</v>
+      </c>
+      <c r="G21" s="1" t="str">
+        <v>YQ</v>
+      </c>
+      <c r="H21" s="1" t="str">
+        <v>BIK</v>
+      </c>
+      <c r="I21" s="1" t="str">
+        <v>DHO</v>
+      </c>
+      <c r="J21" s="1" t="str">
+        <v>FWC</v>
+      </c>
+    </row>
+    <row r="22" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C22" s="1">
+        <v>154</v>
+      </c>
+      <c r="D22" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>EX</v>
+      </c>
+      <c r="F22" s="1" t="str">
+        <v>EX</v>
+      </c>
+      <c r="G22" s="1" t="str">
+        <v>AAB</v>
+      </c>
+      <c r="H22" s="1" t="str">
+        <v>BKP</v>
+      </c>
+      <c r="I22" s="1" t="str">
+        <v>DKN</v>
+      </c>
+      <c r="J22" s="1" t="str">
+        <v>FZV</v>
+      </c>
+    </row>
+    <row r="23" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C23" s="1">
+        <v>172</v>
+      </c>
+      <c r="D23" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>FP</v>
+      </c>
+      <c r="F23" s="1" t="str">
+        <v>FP</v>
+      </c>
+      <c r="G23" s="1" t="str">
+        <v>ABN</v>
+      </c>
+      <c r="H23" s="1" t="str">
+        <v>BMV</v>
+      </c>
+      <c r="I23" s="1" t="str">
+        <v>DNN</v>
+      </c>
+      <c r="J23" s="1" t="str">
+        <v>GDP</v>
+      </c>
+    </row>
+    <row r="24" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C24" s="1">
+        <v>191</v>
+      </c>
+      <c r="D24" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>GI</v>
+      </c>
+      <c r="F24" s="1" t="str">
+        <v>GI</v>
+      </c>
+      <c r="G24" s="1" t="str">
+        <v>ADA</v>
+      </c>
+      <c r="H24" s="1" t="str">
+        <v>BPC</v>
+      </c>
+      <c r="I24" s="1" t="str">
+        <v>DQO</v>
+      </c>
+      <c r="J24" s="1" t="str">
+        <v>GHK</v>
+      </c>
+    </row>
+    <row r="25" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C25" s="1">
+        <v>211</v>
+      </c>
+      <c r="D25" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>HC</v>
+      </c>
+    </row>
+    <row r="26" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C26" s="1">
+        <v>232</v>
+      </c>
+      <c r="D26" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>HX</v>
+      </c>
+      <c r="N26" s="1" t="b" cm="1">
+        <f t="array" ref="N26:R45">_xlfn.ANCHORARRAY(F5)=N1:R20</f>
+        <v>1</v>
+      </c>
+      <c r="O26" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="P26" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="R26" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C27" s="1">
+        <v>254</v>
+      </c>
+      <c r="D27" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>IT</v>
+      </c>
+      <c r="N27" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="O27" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="P27" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q27" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="R27" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C28" s="1">
+        <v>277</v>
+      </c>
+      <c r="D28" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>JQ</v>
+      </c>
+      <c r="N28" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="O28" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="P28" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="R28" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C29" s="1">
+        <v>301</v>
+      </c>
+      <c r="D29" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>KO</v>
+      </c>
+      <c r="N29" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="O29" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="P29" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q29" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="R29" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C30" s="1">
+        <v>326</v>
+      </c>
+      <c r="D30" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>LN</v>
+      </c>
+      <c r="N30" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="O30" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="P30" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q30" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="R30" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C31" s="1">
+        <v>352</v>
+      </c>
+      <c r="D31" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>MN</v>
+      </c>
+      <c r="N31" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="O31" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="P31" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q31" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="R31" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C32" s="1">
+        <v>379</v>
+      </c>
+      <c r="D32" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>NO</v>
+      </c>
+      <c r="N32" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="O32" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="P32" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q32" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="R32" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C33" s="1">
+        <v>407</v>
+      </c>
+      <c r="D33" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>OQ</v>
+      </c>
+      <c r="N33" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="O33" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="P33" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q33" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="R33" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C34" s="1">
+        <v>436</v>
+      </c>
+      <c r="D34" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>PT</v>
+      </c>
+      <c r="N34" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="O34" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="P34" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q34" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="R34" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C35" s="1">
+        <v>466</v>
+      </c>
+      <c r="D35" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>QX</v>
+      </c>
+      <c r="N35" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="O35" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="P35" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q35" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="R35" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C36" s="1">
+        <v>497</v>
+      </c>
+      <c r="D36" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>SC</v>
+      </c>
+      <c r="N36" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="O36" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="P36" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q36" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="R36" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C37" s="1">
+        <v>529</v>
+      </c>
+      <c r="D37" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>TI</v>
+      </c>
+      <c r="N37" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="O37" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="P37" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q37" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="R37" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C38" s="1">
+        <v>562</v>
+      </c>
+      <c r="D38" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>UP</v>
+      </c>
+      <c r="N38" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="O38" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="P38" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q38" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="R38" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C39" s="1">
+        <v>596</v>
+      </c>
+      <c r="D39" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>VX</v>
+      </c>
+      <c r="N39" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="O39" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="P39" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q39" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="R39" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C40" s="1">
+        <v>631</v>
+      </c>
+      <c r="D40" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>XG</v>
+      </c>
+      <c r="N40" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="O40" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="P40" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q40" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="R40" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C41" s="1">
+        <v>667</v>
+      </c>
+      <c r="D41" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>YQ</v>
+      </c>
+      <c r="N41" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="O41" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="P41" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q41" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="R41" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C42" s="1">
+        <v>704</v>
+      </c>
+      <c r="D42" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>AAB</v>
+      </c>
+      <c r="N42" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="O42" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="P42" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q42" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="R42" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C43" s="1">
+        <v>742</v>
+      </c>
+      <c r="D43" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>ABN</v>
+      </c>
+      <c r="N43" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="O43" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="P43" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q43" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="R43" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C44" s="1">
+        <v>781</v>
+      </c>
+      <c r="D44" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>ADA</v>
+      </c>
+      <c r="N44" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="O44" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="P44" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q44" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="R44" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C45" s="1">
+        <v>821</v>
+      </c>
+      <c r="D45" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>AEO</v>
+      </c>
+      <c r="N45" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="O45" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="P45" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q45" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="R45" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C46" s="1">
+        <v>862</v>
+      </c>
+      <c r="D46" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>AGD</v>
+      </c>
+    </row>
+    <row r="47" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C47" s="1">
+        <v>904</v>
+      </c>
+      <c r="D47" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>AHT</v>
+      </c>
+    </row>
+    <row r="48" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C48" s="1">
+        <v>947</v>
+      </c>
+      <c r="D48" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>AJK</v>
+      </c>
+    </row>
+    <row r="49" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C49" s="1">
+        <v>991</v>
+      </c>
+      <c r="D49" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>ALC</v>
+      </c>
+    </row>
+    <row r="50" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C50" s="1">
+        <v>1036</v>
+      </c>
+      <c r="D50" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>AMV</v>
+      </c>
+    </row>
+    <row r="51" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C51" s="1">
+        <v>1082</v>
+      </c>
+      <c r="D51" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>AOP</v>
+      </c>
+    </row>
+    <row r="52" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C52" s="1">
+        <v>1129</v>
+      </c>
+      <c r="D52" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>AQK</v>
+      </c>
+    </row>
+    <row r="53" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C53" s="1">
+        <v>1177</v>
+      </c>
+      <c r="D53" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>ASG</v>
+      </c>
+    </row>
+    <row r="54" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C54" s="1">
+        <v>1226</v>
+      </c>
+      <c r="D54" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>AUD</v>
+      </c>
+    </row>
+    <row r="55" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C55" s="1">
+        <v>1276</v>
+      </c>
+      <c r="D55" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>AWB</v>
+      </c>
+    </row>
+    <row r="56" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C56" s="1">
+        <v>1327</v>
+      </c>
+      <c r="D56" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>AYA</v>
+      </c>
+    </row>
+    <row r="57" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C57" s="1">
+        <v>1379</v>
+      </c>
+      <c r="D57" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>BAA</v>
+      </c>
+    </row>
+    <row r="58" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C58" s="1">
+        <v>1432</v>
+      </c>
+      <c r="D58" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>BCB</v>
+      </c>
+    </row>
+    <row r="59" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C59" s="1">
+        <v>1486</v>
+      </c>
+      <c r="D59" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>BED</v>
+      </c>
+    </row>
+    <row r="60" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C60" s="1">
+        <v>1541</v>
+      </c>
+      <c r="D60" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>BGG</v>
+      </c>
+    </row>
+    <row r="61" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C61" s="1">
+        <v>1597</v>
+      </c>
+      <c r="D61" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>BIK</v>
+      </c>
+    </row>
+    <row r="62" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C62" s="1">
+        <v>1654</v>
+      </c>
+      <c r="D62" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>BKP</v>
+      </c>
+    </row>
+    <row r="63" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C63" s="1">
+        <v>1712</v>
+      </c>
+      <c r="D63" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>BMV</v>
+      </c>
+    </row>
+    <row r="64" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C64" s="1">
+        <v>1771</v>
+      </c>
+      <c r="D64" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>BPC</v>
+      </c>
+    </row>
+    <row r="65" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C65" s="1">
+        <v>1831</v>
+      </c>
+      <c r="D65" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>BRK</v>
+      </c>
+    </row>
+    <row r="66" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C66" s="1">
+        <v>1892</v>
+      </c>
+      <c r="D66" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>BTT</v>
+      </c>
+    </row>
+    <row r="67" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C67" s="1">
+        <v>1954</v>
+      </c>
+      <c r="D67" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>BWD</v>
+      </c>
+    </row>
+    <row r="68" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C68" s="1">
+        <v>2017</v>
+      </c>
+      <c r="D68" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>BYO</v>
+      </c>
+    </row>
+    <row r="69" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C69" s="1">
+        <v>2081</v>
+      </c>
+      <c r="D69" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CBA</v>
+      </c>
+    </row>
+    <row r="70" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C70" s="1">
+        <v>2146</v>
+      </c>
+      <c r="D70" s="1" t="str">
+        <f t="shared" ref="D70:D104" si="1">SUBSTITUTE(ADDRESS(1,C70,4),"1","")</f>
+        <v>CDN</v>
+      </c>
+    </row>
+    <row r="71" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C71" s="1">
+        <v>2212</v>
+      </c>
+      <c r="D71" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>CGB</v>
+      </c>
+    </row>
+    <row r="72" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C72" s="1">
+        <v>2279</v>
+      </c>
+      <c r="D72" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>CIQ</v>
+      </c>
+    </row>
+    <row r="73" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C73" s="1">
+        <v>2347</v>
+      </c>
+      <c r="D73" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>CLG</v>
+      </c>
+    </row>
+    <row r="74" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C74" s="1">
+        <v>2416</v>
+      </c>
+      <c r="D74" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>CNX</v>
+      </c>
+    </row>
+    <row r="75" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C75" s="1">
+        <v>2486</v>
+      </c>
+      <c r="D75" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>CQP</v>
+      </c>
+    </row>
+    <row r="76" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C76" s="1">
+        <v>2557</v>
+      </c>
+      <c r="D76" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>CTI</v>
+      </c>
+    </row>
+    <row r="77" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C77" s="1">
+        <v>2629</v>
+      </c>
+      <c r="D77" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>CWC</v>
+      </c>
+    </row>
+    <row r="78" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C78" s="1">
+        <v>2702</v>
+      </c>
+      <c r="D78" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>CYX</v>
+      </c>
+    </row>
+    <row r="79" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C79" s="1">
+        <v>2776</v>
+      </c>
+      <c r="D79" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>DBT</v>
+      </c>
+    </row>
+    <row r="80" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C80" s="1">
+        <v>2851</v>
+      </c>
+      <c r="D80" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>DEQ</v>
+      </c>
+    </row>
+    <row r="81" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C81" s="1">
+        <v>2927</v>
+      </c>
+      <c r="D81" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>DHO</v>
+      </c>
+    </row>
+    <row r="82" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C82" s="1">
+        <v>3004</v>
+      </c>
+      <c r="D82" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>DKN</v>
+      </c>
+    </row>
+    <row r="83" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C83" s="1">
+        <v>3082</v>
+      </c>
+      <c r="D83" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>DNN</v>
+      </c>
+    </row>
+    <row r="84" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C84" s="1">
+        <v>3161</v>
+      </c>
+      <c r="D84" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>DQO</v>
+      </c>
+    </row>
+    <row r="85" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C85" s="1">
+        <v>3241</v>
+      </c>
+      <c r="D85" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>DTQ</v>
+      </c>
+    </row>
+    <row r="86" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C86" s="1">
+        <v>3322</v>
+      </c>
+      <c r="D86" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>DWT</v>
+      </c>
+    </row>
+    <row r="87" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C87" s="1">
+        <v>3404</v>
+      </c>
+      <c r="D87" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>DZX</v>
+      </c>
+    </row>
+    <row r="88" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C88" s="1">
+        <v>3487</v>
+      </c>
+      <c r="D88" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>EDC</v>
+      </c>
+    </row>
+    <row r="89" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C89" s="1">
+        <v>3571</v>
+      </c>
+      <c r="D89" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>EGI</v>
+      </c>
+    </row>
+    <row r="90" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C90" s="1">
+        <v>3656</v>
+      </c>
+      <c r="D90" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>EJP</v>
+      </c>
+    </row>
+    <row r="91" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C91" s="1">
+        <v>3742</v>
+      </c>
+      <c r="D91" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>EMX</v>
+      </c>
+    </row>
+    <row r="92" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C92" s="1">
+        <v>3829</v>
+      </c>
+      <c r="D92" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>EQG</v>
+      </c>
+    </row>
+    <row r="93" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C93" s="1">
+        <v>3917</v>
+      </c>
+      <c r="D93" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>ETQ</v>
+      </c>
+    </row>
+    <row r="94" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C94" s="1">
+        <v>4006</v>
+      </c>
+      <c r="D94" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>EXB</v>
+      </c>
+    </row>
+    <row r="95" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C95" s="1">
+        <v>4096</v>
+      </c>
+      <c r="D95" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>FAN</v>
+      </c>
+    </row>
+    <row r="96" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C96" s="1">
+        <v>4187</v>
+      </c>
+      <c r="D96" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>FEA</v>
+      </c>
+    </row>
+    <row r="97" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C97" s="1">
+        <v>4279</v>
+      </c>
+      <c r="D97" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>FHO</v>
+      </c>
+    </row>
+    <row r="98" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C98" s="1">
+        <v>4372</v>
+      </c>
+      <c r="D98" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>FLD</v>
+      </c>
+    </row>
+    <row r="99" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C99" s="1">
+        <v>4466</v>
+      </c>
+      <c r="D99" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>FOT</v>
+      </c>
+    </row>
+    <row r="100" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C100" s="1">
+        <v>4561</v>
+      </c>
+      <c r="D100" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>FSK</v>
+      </c>
+    </row>
+    <row r="101" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C101" s="1">
+        <v>4657</v>
+      </c>
+      <c r="D101" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>FWC</v>
+      </c>
+    </row>
+    <row r="102" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C102" s="1">
+        <v>4754</v>
+      </c>
+      <c r="D102" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>FZV</v>
+      </c>
+    </row>
+    <row r="103" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C103" s="1">
+        <v>4852</v>
+      </c>
+      <c r="D103" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>GDP</v>
+      </c>
+    </row>
+    <row r="104" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C104" s="1">
+        <v>4951</v>
+      </c>
+      <c r="D104" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>GHK</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACD76393-EAAF-4FD6-9CBA-7F673827FCCB}">
   <dimension ref="A1:ALL12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10:E12"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
@@ -7032,13 +8885,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0B61FB7-2A3F-43AC-901D-9F2BA37AFCFE}">
   <dimension ref="A2:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5:D8"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>

</xml_diff>